<commit_message>
append column names to sheet
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Diagnoses" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,12 +424,67 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>Id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>world!</t>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Temperature</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Symptoms</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Total Ulhi</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Total Serious</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Total Common</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Total Less Common</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Current Fever</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Result</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
diagnoses from db to excel complete
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,108 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>demo@email.com</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>109.4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>23</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Loss of Movement,Fever,Tiredness</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jake</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>demo@email.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="F3" t="n">
+        <v>34</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Tiredness</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
button added to main screen to generate xlsx and email it
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,6 +590,57 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>demo@email.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>107.6</v>
+      </c>
+      <c r="F4" t="n">
+        <v>19</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Chest Pain,Loss of Movement,Fever,Dry Cough,Aches,Sore Throat</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
individual emails now being sent with results after diagnosis
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -692,6 +692,261 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kai</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Havertz</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>21</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Chest Pain,Loss of Speech,Tiredness,Pains</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>21</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Chest Pain,Loss of Movement,Dry Cough,Aches</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>jt@eml.com</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>32</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Chest Pain,Fever,Dry Cough,Tiredness</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>jandoe@email.com</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>23</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Chest Pain,Loss of Movement,Dry Cough,Pains</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Chad-Allan</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Oliver</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>21</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Chest Pain,Fever,Dry Cough,Tiredness</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
persist underlying health issues to db & excel
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,45 +459,50 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>Underlying Health Issues</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>Total Ulhi</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Total Serious</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Total Common</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Total Less Common</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Diastolic Val</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Systolic Val</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Low Bp</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Current Fever</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Result</t>
         </is>
@@ -509,12 +514,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Chad</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -523,41 +528,233 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>104</v>
+        <v>96.8</v>
       </c>
       <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Pains</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Asthma</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Oliver</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>100.4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Asthma</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Oliver</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>100.4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>blank</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Asthma</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Oliver</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>109.4</v>
+      </c>
+      <c r="F5" t="n">
         <v>21</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Chest Pain,Dry Cough,Aches,Conjunctivitis,Loss of Smell</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Chest Pain,Loss of Speech</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
         <v>2</v>
       </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="inlineStr">
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Very High Risk</t>
         </is>

</xml_diff>

<commit_message>
added check for spike value (WIP) and sends alert email to admin
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -528,23 +528,19 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>96.8</v>
+        <v>96.98</v>
       </c>
       <c r="F2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Pains</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>Asthma</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -553,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -593,28 +589,32 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>100.4</v>
+        <v>102.2</v>
       </c>
       <c r="F3" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Chest Pain,Fever,Aches,Sore Throat</t>
+        </is>
+      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Asthma,Dementia</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>Not at Risk</t>
+          <t>Very High Risk</t>
         </is>
       </c>
     </row>
@@ -640,12 +640,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>Jane</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Oliver</t>
+          <t>Doe</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -654,32 +654,32 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>100.4</v>
+        <v>116.6</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>blank</t>
+          <t>Difficulty Breathing,Fever,Tiredness,Sore Throat,Conjunctivitis,Headache</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Asthma</t>
+          <t>Cancer,Asthma,Pulmonary Hypertension,Dementia</t>
         </is>
       </c>
       <c r="I4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" t="n">
         <v>1</v>
       </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -695,7 +695,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Not at Risk</t>
+          <t>Very High Risk</t>
         </is>
       </c>
     </row>
@@ -705,12 +705,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>Cha</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Oliver</t>
+          <t>O</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -719,25 +719,29 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>109.4</v>
+        <v>111.2</v>
       </c>
       <c r="F5" t="n">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Chest Pain,Loss of Speech</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>Difficulty Breathing,Loss of Movement,Fever</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Asthma,Pulmonary Hypertension</t>
+        </is>
+      </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
         <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
alert feature done (needs to be tested, but should be fully working.)
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,12 +528,16 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>96.98</v>
+        <v>113</v>
       </c>
       <c r="F2" t="n">
         <v>20</v>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Chest Pain,Loss of Movement,Fever,Tiredness,Pains,Sore Throat</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>Asthma</t>
@@ -543,13 +547,13 @@
         <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -564,201 +568,6 @@
         <v>0</v>
       </c>
       <c r="Q2" t="inlineStr">
-        <is>
-          <t>Not at Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Chad</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Oliver</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>chadoliver017@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>102.2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>20</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Chest Pain,Fever,Aches,Sore Throat</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Asthma,Dementia</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Very High Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Jane</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Doe</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>chadoliver017@gmail.com</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>116.6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>68</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Difficulty Breathing,Fever,Tiredness,Sore Throat,Conjunctivitis,Headache</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Cancer,Asthma,Pulmonary Hypertension,Dementia</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>4</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" t="n">
-        <v>3</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="b">
-        <v>0</v>
-      </c>
-      <c r="P4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Very High Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cha</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>chadoliver017@gmail.com</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>111.2</v>
-      </c>
-      <c r="F5" t="n">
-        <v>90</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Difficulty Breathing,Loss of Movement,Fever</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Asthma,Pulmonary Hypertension</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="inlineStr">
         <is>
           <t>Very High Risk</t>
         </is>

</xml_diff>

<commit_message>
clear db feature done & diagnose prolog function updated
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,12 +514,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Chad</t>
+          <t>John</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Oliver</t>
+          <t>Doe</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,46 +528,111 @@
         </is>
       </c>
       <c r="E2" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>65</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Chest Pain,Pressure,Fever,Tiredness</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Chronic Kidney Disease,Asthma,Dementia</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jane</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>chadoliver017@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>113</v>
       </c>
-      <c r="F2" t="n">
-        <v>20</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Difficulty Breathing,Chest Pain,Loss of Movement,Fever,Tiredness,Pains,Sore Throat</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Asthma</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+      <c r="F3" t="n">
+        <v>68</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Pressure,Fever,Pains,Headache,Loss of Taste,Discolouration</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Cancer,Cystic Fibrosis,Dementia,Down syndrome</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" t="n">
         <v>1</v>
       </c>
-      <c r="J2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K2" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="b">
-        <v>0</v>
-      </c>
-      <c r="P2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="inlineStr">
+      <c r="L3" t="n">
+        <v>4</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Very High Risk</t>
         </is>

</xml_diff>

<commit_message>
added modal confirmation dialogs + removed current fever text (swapped for temperature)
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -514,12 +514,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Chad</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -528,26 +528,26 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>111.2</v>
+        <v>113</v>
       </c>
       <c r="F2" t="n">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Chest Pain,Pressure,Fever,Tiredness</t>
+          <t>Chest Pain,Fever</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Chronic Kidney Disease,Asthma,Dementia</t>
+          <t>Asthma</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -579,12 +579,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jane</t>
+          <t>Chad</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Doe</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -593,32 +593,32 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>113</v>
+        <v>118.4</v>
       </c>
       <c r="F3" t="n">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Difficulty Breathing,Pressure,Fever,Pains,Headache,Loss of Taste,Discolouration</t>
+          <t>Chest Pain,Fever</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cancer,Cystic Fibrosis,Dementia,Down syndrome</t>
+          <t>Asthma</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
fix merge issue for clear db branch
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,6 +573,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dave</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robinson </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Error & Success Message/Restricted Submit
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,6 +573,661 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dave</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robinson </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Dave</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Robinson</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>95</v>
+      </c>
+      <c r="F4" t="n">
+        <v>24</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>j</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>95</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>95</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>86</v>
+      </c>
+      <c r="F7" t="n">
+        <v>54</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Dave</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Robinson </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>95</v>
+      </c>
+      <c r="F8" t="n">
+        <v>26</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>r</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>136.4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>60</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Chest Pain,Fever,Dry Cough,Tiredness,Aches,Pains,Sore Throat</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Asthma,Dementia</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" t="n">
+        <v>3</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>152.6</v>
+      </c>
+      <c r="F10" t="n">
+        <v>78</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Difficulty Breathing,Chest Pain,Pressure,Fever,Dry Cough,Tiredness,Aches,Pains,Sore Throat</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Asthma,Pulmonary Hypertension</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>3</v>
+      </c>
+      <c r="L10" t="n">
+        <v>3</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Very High Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>86</v>
+      </c>
+      <c r="F11" t="n">
+        <v>23</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Dry Cough,Sore Throat</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <v>0</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="F12" t="n">
+        <v>23</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Fever,Dry Cough,Pains,Sore Throat</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>R</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="F13" t="n">
+        <v>23</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Chest Pain,Fever,Dry Cough,Pains</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Asthma</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Not at Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add lowbp symtoms to be checked
</commit_message>
<xml_diff>
--- a/data/diagnoses.xlsx
+++ b/data/diagnoses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1228,6 +1228,189 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Otra</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Baker</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>113</v>
+      </c>
+      <c r="F14" t="n">
+        <v>34</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Aches</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Otra</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Baker</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yaho..com</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>113</v>
+      </c>
+      <c r="F15" t="n">
+        <v>34</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Aches</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Otra</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Baker</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>robinsondave_876@yahoo.com</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>113</v>
+      </c>
+      <c r="F16" t="n">
+        <v>34</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Aches</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="b">
+        <v>0</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Low Risk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>